<commit_message>
extra update for Version 2 model
</commit_message>
<xml_diff>
--- a/EEG_Dassl_Lightning/analyze_experiment/NeurIPS/data/experiment_3.xlsx
+++ b/EEG_Dassl_Lightning/analyze_experiment/NeurIPS/data/experiment_3.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,19 +571,19 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.513</v>
+        <v>0.506</v>
       </c>
       <c r="F4" t="n">
-        <v>0.45</v>
+        <v>0.431</v>
       </c>
       <c r="G4" t="n">
-        <v>0.375</v>
+        <v>0.456</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5</v>
+        <v>0.469</v>
       </c>
       <c r="I4" t="n">
-        <v>0.463</v>
+        <v>0.419</v>
       </c>
     </row>
     <row r="5">
@@ -592,110 +592,102 @@
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>base</t>
+          <t>adaptV1</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.331</v>
+        <v>0.587</v>
       </c>
       <c r="F5" t="n">
-        <v>0.356</v>
+        <v>0.569</v>
       </c>
       <c r="G5" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
       <c r="H5" t="n">
-        <v>0.325</v>
+        <v>0.487</v>
       </c>
       <c r="I5" t="n">
-        <v>0.337</v>
+        <v>0.469</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>temp</t>
-        </is>
-      </c>
+      <c r="C6" s="1" t="n"/>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>adapt</t>
+          <t>base</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.531</v>
+        <v>0.275</v>
       </c>
       <c r="F6" t="n">
-        <v>0.456</v>
+        <v>0.344</v>
       </c>
       <c r="G6" t="n">
-        <v>0.413</v>
+        <v>0.356</v>
       </c>
       <c r="H6" t="n">
-        <v>0.481</v>
+        <v>0.269</v>
       </c>
       <c r="I6" t="n">
-        <v>0.406</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>base</t>
+          <t>adapt</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.344</v>
+        <v>0.375</v>
       </c>
       <c r="F7" t="n">
-        <v>0.281</v>
+        <v>0.513</v>
       </c>
       <c r="G7" t="n">
-        <v>0.306</v>
+        <v>0.331</v>
       </c>
       <c r="H7" t="n">
-        <v>0.419</v>
+        <v>0.444</v>
       </c>
       <c r="I7" t="n">
-        <v>0.281</v>
+        <v>0.462</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>adapt</t>
+          <t>adaptV1</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.356</v>
+        <v>0.594</v>
       </c>
       <c r="F8" t="n">
-        <v>0.431</v>
+        <v>0.587</v>
       </c>
       <c r="G8" t="n">
-        <v>0.431</v>
+        <v>0.531</v>
       </c>
       <c r="H8" t="n">
-        <v>0.344</v>
+        <v>0.55</v>
       </c>
       <c r="I8" t="n">
-        <v>0.406</v>
+        <v>0.419</v>
       </c>
     </row>
     <row r="9">
@@ -708,27 +700,31 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.45</v>
+        <v>0.281</v>
       </c>
       <c r="F9" t="n">
-        <v>0.325</v>
+        <v>0.381</v>
       </c>
       <c r="G9" t="n">
-        <v>0.319</v>
+        <v>0.337</v>
       </c>
       <c r="H9" t="n">
-        <v>0.212</v>
+        <v>0.294</v>
       </c>
       <c r="I9" t="n">
-        <v>0.269</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>no</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
@@ -737,19 +733,19 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.444</v>
+        <v>0.475</v>
       </c>
       <c r="F10" t="n">
-        <v>0.275</v>
+        <v>0.475</v>
       </c>
       <c r="G10" t="n">
-        <v>0.431</v>
+        <v>0.344</v>
       </c>
       <c r="H10" t="n">
-        <v>0.456</v>
+        <v>0.506</v>
       </c>
       <c r="I10" t="n">
-        <v>0.419</v>
+        <v>0.438</v>
       </c>
     </row>
     <row r="11">
@@ -758,114 +754,102 @@
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="1" t="inlineStr">
         <is>
+          <t>adaptV1</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.356</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.325</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
           <t>base</t>
         </is>
       </c>
-      <c r="E11" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.487</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.388</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I11" t="n">
+      <c r="E12" t="n">
+        <v>0.231</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.306</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>dataset_B</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>chan</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="D12" s="1" t="inlineStr">
-        <is>
-          <t>adapt</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>0.549</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.531</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.51</v>
-      </c>
       <c r="H12" t="n">
-        <v>0.514</v>
+        <v>0.225</v>
       </c>
       <c r="I12" t="n">
-        <v>0.556</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
-          <t>base</t>
+          <t>adapt</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.448</v>
+        <v>0.481</v>
       </c>
       <c r="F13" t="n">
-        <v>0.276</v>
+        <v>0.487</v>
       </c>
       <c r="G13" t="n">
-        <v>0.333</v>
+        <v>0.431</v>
       </c>
       <c r="H13" t="n">
-        <v>0.385</v>
+        <v>0.494</v>
       </c>
       <c r="I13" t="n">
-        <v>0.365</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>temp</t>
-        </is>
-      </c>
+      <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
-          <t>adapt</t>
+          <t>adaptV1</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.528</v>
+        <v>0.3</v>
       </c>
       <c r="F14" t="n">
-        <v>0.59</v>
+        <v>0.469</v>
       </c>
       <c r="G14" t="n">
-        <v>0.521</v>
+        <v>0.356</v>
       </c>
       <c r="H14" t="n">
-        <v>0.493</v>
+        <v>0.25</v>
       </c>
       <c r="I14" t="n">
-        <v>0.587</v>
+        <v>0.337</v>
       </c>
     </row>
     <row r="15">
@@ -878,52 +862,56 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.453</v>
+        <v>0.337</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5</v>
+        <v>0.419</v>
       </c>
       <c r="G15" t="n">
-        <v>0.479</v>
+        <v>0.381</v>
       </c>
       <c r="H15" t="n">
-        <v>0.531</v>
+        <v>0.569</v>
       </c>
       <c r="I15" t="n">
-        <v>0.49</v>
+        <v>0.319</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n"/>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>dataset_B</t>
+        </is>
+      </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
+          <t>chan</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
           <t>adapt</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.51</v>
+        <v>0.497</v>
       </c>
       <c r="F16" t="n">
-        <v>0.514</v>
+        <v>0.521</v>
       </c>
       <c r="G16" t="n">
-        <v>0.535</v>
+        <v>0.497</v>
       </c>
       <c r="H16" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.538</v>
       </c>
       <c r="I16" t="n">
-        <v>0.608</v>
+        <v>0.573</v>
       </c>
     </row>
     <row r="17">
@@ -932,96 +920,308 @@
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>base</t>
+          <t>adaptV1</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.401</v>
+        <v>0.535</v>
       </c>
       <c r="F17" t="n">
-        <v>0.365</v>
+        <v>0.542</v>
       </c>
       <c r="G17" t="n">
-        <v>0.349</v>
+        <v>0.604</v>
       </c>
       <c r="H17" t="n">
-        <v>0.391</v>
+        <v>0.618</v>
       </c>
       <c r="I17" t="n">
-        <v>0.51</v>
+        <v>0.583</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>temp</t>
-        </is>
-      </c>
+      <c r="C18" s="1" t="n"/>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>adapt</t>
+          <t>base</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.458</v>
+        <v>0.37</v>
       </c>
       <c r="F18" t="n">
-        <v>0.517</v>
+        <v>0.344</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5620000000000001</v>
+        <v>0.396</v>
       </c>
       <c r="H18" t="n">
-        <v>0.587</v>
+        <v>0.255</v>
       </c>
       <c r="I18" t="n">
-        <v>0.597</v>
+        <v>0.406</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="n"/>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
+          <t>adapt</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0.542</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.573</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>adaptV1</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0.538</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.608</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.594</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.611</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
           <t>base</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>0.453</v>
-      </c>
-      <c r="F19" t="n">
+      <c r="E21" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.573</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.651</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.542</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>adapt</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.521</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.601</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.601</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.5590000000000001</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>adaptV1</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0.521</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.517</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>base</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
         <v>0.401</v>
       </c>
-      <c r="G19" t="n">
+      <c r="F24" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.458</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>adapt</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
         <v>0.479</v>
       </c>
-      <c r="H19" t="n">
-        <v>0.547</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.5679999999999999</v>
+      <c r="F25" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.587</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.587</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>adaptV1</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0.521</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.399</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.556</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="n"/>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>base</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0.526</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.437</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.443</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.542</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.589</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A4:A15"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>